<commit_message>
Added symbols, formatted frontpage and formatted percentage plotting
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Key-Insight.xlsx
+++ b/TIMES_shiny/data_cleaning/Key-Insight.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
   <si>
     <t>Parameter</t>
   </si>
@@ -66,6 +66,24 @@
   </si>
   <si>
     <t>Million tonnes CO2 equivalent (MtCO2-e)</t>
+  </si>
+  <si>
+    <t>Kea renewable</t>
+  </si>
+  <si>
+    <t>Tui renewable</t>
+  </si>
+  <si>
+    <t>Kea Renewable energy</t>
+  </si>
+  <si>
+    <t>Tui Renewable energy</t>
+  </si>
+  <si>
+    <t>Kea Electrification</t>
+  </si>
+  <si>
+    <t>Tui Electrification</t>
   </si>
 </sst>
 </file>
@@ -403,14 +421,14 @@
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -745,7 +763,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -794,8 +812,8 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -845,7 +863,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -895,7 +913,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
@@ -944,8 +962,8 @@
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>3</v>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
@@ -994,8 +1012,8 @@
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Update to Key Insights
Label change - error fix in last update
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Key-Insight.xlsx
+++ b/TIMES_shiny/data_cleaning/Key-Insight.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
   <si>
     <t>Parameter</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Electrification Percentage</t>
+  </si>
+  <si>
+    <t>Renewable Energy Percentage</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,10 +943,10 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
@@ -990,10 +993,10 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Fixed Anand's comment; About page, Over and assumption stuff
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Key-Insight.xlsx
+++ b/TIMES_shiny/data_cleaning/Key-Insight.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
   <si>
     <t>Parameter</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t xml:space="preserve">Electrification </t>
+  </si>
+  <si>
+    <t>All energy related cumulative emissions</t>
+  </si>
+  <si>
+    <t>All energy related annual emissions</t>
+  </si>
+  <si>
+    <t>Electricity generation from solar</t>
+  </si>
+  <si>
+    <t>Transport emissions</t>
+  </si>
+  <si>
+    <t>Industrial emissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renewable electricity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renewable energy </t>
   </si>
 </sst>
 </file>
@@ -413,7 +434,7 @@
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +488,7 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -507,8 +528,8 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -549,7 +570,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -598,8 +619,8 @@
       <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
+      <c r="A5" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -649,7 +670,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -706,7 +727,7 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -763,7 +784,7 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -813,7 +834,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -863,7 +884,7 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -913,7 +934,7 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -963,7 +984,7 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
@@ -1013,7 +1034,7 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1063,7 +1084,7 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
@@ -1113,7 +1134,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>

</xml_diff>